<commit_message>
Updated win achievement points
</commit_message>
<xml_diff>
--- a/My Sets/Checkers (Fairchild Channel F)/Checkers - Plan.xlsx
+++ b/My Sets/Checkers (Fairchild Channel F)/Checkers - Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="2" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>Win a game by capturing all of the opponents pieces in 50 turns or less</t>
   </si>
   <si>
-    <t>46 best so far</t>
-  </si>
-  <si>
     <t>Sacrifice a piece to capture two or more pieces in a single trade</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>Quick Winner!</t>
+  </si>
+  <si>
+    <t>26 best so far</t>
   </si>
 </sst>
 </file>
@@ -661,8 +661,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -819,7 +819,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>16</v>
@@ -829,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -841,7 +841,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -863,7 +863,7 @@
         <v>33</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
@@ -907,7 +907,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>11</v>
@@ -917,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -929,7 +929,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>11</v>
@@ -939,7 +939,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -983,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1025,7 +1025,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>25</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="7"/>
     </row>
@@ -1080,17 +1080,17 @@
         <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="7">
         <f>VLOOKUP(D19,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1104,17 +1104,17 @@
         <v>51</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="7">
         <f>VLOOKUP(D20,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1125,20 +1125,20 @@
         <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="E21" s="7">
         <f>VLOOKUP(D21,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2130,7 +2130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2170,26 +2170,26 @@
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3111,19 +3111,19 @@
     <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Decisive Victory!","Win a game by capturing all of the opponents pieces in 65 turns or less", 10, trigger)</v>
+        <v>achievement("Decisive Victory!","Win a game by capturing all of the opponents pieces in 65 turns or less", 5, trigger)</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Quick Victory!","Win a game by capturing all of the opponents pieces in 50 turns or less", 25, trigger)</v>
+        <v>achievement("Quick Victory!","Win a game by capturing all of the opponents pieces in 50 turns or less", 10, trigger)</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Absolute Victory!","Win a game by capturing all of the opponents pieces in 40 turns or less", 50, trigger)</v>
+        <v>achievement("Absolute Victory!","Win a game by capturing all of the opponents pieces in 40 turns or less", 25, trigger)</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="G4" s="7">
         <f>SUMIF(Achievements!B:B,E4,Achievements!E:E)</f>
-        <v>153</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Achievements!D:D,A7)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>170</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3665,7 +3665,7 @@
       </c>
       <c r="C10">
         <f>COUNTIF(Achievements!D:D,A10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reduced turn limits for checkers
</commit_message>
<xml_diff>
--- a/My Sets/Checkers (Fairchild Channel F)/Checkers - Plan.xlsx
+++ b/My Sets/Checkers (Fairchild Channel F)/Checkers - Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\RetroArch\Achievements\Checkers (Fairchild Channel F)\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egrea\Dropbox\RetroArch\Achievements\Checkers (Fairchild Channel F)\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -233,9 +233,6 @@
     <t>Win a game by blocking the opponent from moving</t>
   </si>
   <si>
-    <t>Win a game by capturing all of the opponents pieces in 65 turns or less</t>
-  </si>
-  <si>
     <t>Decisive Victory!</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>26 best so far</t>
+  </si>
+  <si>
+    <t>Win a game by capturing all of the opponents pieces in 30 turns or less</t>
   </si>
 </sst>
 </file>
@@ -661,8 +661,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +819,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>16</v>
@@ -829,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -841,7 +841,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -917,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -929,7 +929,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>11</v>
@@ -939,7 +939,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -983,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1025,7 +1025,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>11</v>
@@ -1090,7 +1090,7 @@
         <v>5</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1111,10 +1111,10 @@
         <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1125,7 +1125,7 @@
         <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>13</v>
@@ -1135,10 +1135,10 @@
         <v>25</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2170,26 +2170,26 @@
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="C19" s="7" t="str">
         <f>Achievements!F19</f>
-        <v>Win a game by capturing all of the opponents pieces in 65 turns or less</v>
+        <v>Win a game by capturing all of the opponents pieces in 50 turns or less</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>19</v>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="C20" s="7" t="str">
         <f>Achievements!F20</f>
-        <v>Win a game by capturing all of the opponents pieces in 50 turns or less</v>
+        <v>Win a game by capturing all of the opponents pieces in 40 turns or less</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>19</v>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="C21" s="7" t="str">
         <f>Achievements!F21</f>
-        <v>Win a game by capturing all of the opponents pieces in 40 turns or less</v>
+        <v>Win a game by capturing all of the opponents pieces in 30 turns or less</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>19</v>
@@ -3111,19 +3111,19 @@
     <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Decisive Victory!","Win a game by capturing all of the opponents pieces in 65 turns or less", 5, trigger)</v>
+        <v>achievement("Decisive Victory!","Win a game by capturing all of the opponents pieces in 50 turns or less", 5, trigger)</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Quick Victory!","Win a game by capturing all of the opponents pieces in 50 turns or less", 10, trigger)</v>
+        <v>achievement("Quick Victory!","Win a game by capturing all of the opponents pieces in 40 turns or less", 10, trigger)</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Absolute Victory!","Win a game by capturing all of the opponents pieces in 40 turns or less", 25, trigger)</v>
+        <v>achievement("Absolute Victory!","Win a game by capturing all of the opponents pieces in 30 turns or less", 25, trigger)</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>